<commit_message>
07-05-2024 | Introduction to server building
</commit_message>
<xml_diff>
--- a/products.xlsx
+++ b/products.xlsx
@@ -397,7 +397,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:B11"/>
+  <dimension ref="A1:A17"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -406,93 +406,90 @@
       <c r="A1" t="str">
         <v>name</v>
       </c>
-      <c r="B1" t="str">
-        <v>price</v>
-      </c>
     </row>
     <row r="2">
       <c r="A2" t="str">
-        <v>IPhone</v>
-      </c>
-      <c r="B2" t="str">
-        <v>99999</v>
+        <v>Redmi 13C (Starfrost White, 4GB RAM, 128GB Storage) | Powered by 4G MediaTek Helio G85 | 90Hz Display | 50MP AI Triple Camera</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="str">
-        <v>Samsung galaxy s24</v>
-      </c>
-      <c r="B3" t="str">
-        <v>79999</v>
+        <v>Samsung Galaxy M14 5G (Smoky Teal,6GB,128GB)|50MP Triple Cam|Segment's Only 6000 mAh 5G SP|5nm Processor|2 Gen. OS Upgrade &amp; 4 Year Security Update|12GB RAM with RAM Plus|Android 13|Without Charger</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="str">
-        <v>Samsung galaxy s24</v>
-      </c>
-      <c r="B4" t="str">
-        <v>79999</v>
+        <v>Redmi 13C (Stardust Black, 6GB RAM, 128GB Storage) | Powered by 4G MediaTek Helio G85 | 90Hz Display | 50MP AI Triple Camera</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="str">
-        <v>Samsung galaxy s24</v>
-      </c>
-      <c r="B5" t="str">
-        <v>79999</v>
+        <v>Redmi 13C (Starshine Green, 4GB RAM, 128GB Storage) | Powered by 4G MediaTek Helio G85 | 90Hz Display | 50MP AI Triple Camera</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="str">
-        <v>Samsung galaxy s24</v>
-      </c>
-      <c r="B6" t="str">
-        <v>79999</v>
+        <v>realme NARZO 70x 5G (Forest Green,4GB RAM, 128GB Storage) |120Hz Ultra Smooth Display | Dimensity 6100+ 6nm 5G | 50MP AI Camera|45W Charger in The Box</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="str">
-        <v>Samsung galaxy s24</v>
-      </c>
-      <c r="B7" t="str">
-        <v>79999</v>
+        <v>POCO C65 Matte Black 4GB RAM 128GB ROM</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="str">
-        <v>Samsung galaxy s24</v>
-      </c>
-      <c r="B8" t="str">
-        <v>79999</v>
+        <v>iQOO Z6 Lite 5G (Stellar Green, 6GB RAM, 128GB Storage) with Charger | Qualcomm Snapdragon 4 Gen 1 Processor | 120Hz FHD+ Display | Travel Adaptor Included in The Box</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="str">
-        <v>Samsung galaxy s24</v>
-      </c>
-      <c r="B9" t="str">
-        <v>79999</v>
+        <v>realme narzo N53 (Feather Black, 4GB+64GB) 33W Segment Fastest Charging | Slim Smartphone | 90 Hz Smooth Display</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="str">
-        <v>Samsung galaxy s24</v>
-      </c>
-      <c r="B10" t="str">
-        <v>79999</v>
+        <v>TECNO POP 8 (Gravity Black,(8GB*+64GB)| 90Hz Punch Hole Display with Dynamic Port &amp; Dual Speakers with DTS| 5000mAh Battery |10W Type-C| Side Fingerprint Sensor| Octa-Core Processor</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="str">
-        <v>Samsung galaxy s24</v>
-      </c>
-      <c r="B11" t="str">
-        <v>79999</v>
+        <v>OnePlus Nord CE 3 5G (Aqua Surge, 8GB RAM, 128GB Storage)</v>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" t="str">
+        <v>Redmi 12 5G Jade Black 6GB RAM 128GB ROM</v>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" t="str">
+        <v>realme narzo 60X 5G (Stellar Green,6GB,128GB Storage) Up to 2TB External Memory | 50 MP AI Primary Camera | Segments only 33W Supervooc Charge</v>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14" t="str">
+        <v>OnePlus Nord CE 3 Lite 5G (Chromatic Gray, 8GB RAM, 256GB Storage)</v>
+      </c>
+    </row>
+    <row r="15">
+      <c r="A15" t="str">
+        <v>Redmi 13C (Starfrost White, 6GB RAM, 128GB Storage) | Powered by 4G MediaTek Helio G85 | 90Hz Display | 50MP AI Triple Camera</v>
+      </c>
+    </row>
+    <row r="16">
+      <c r="A16" t="str">
+        <v>POCO C65 Pastel Blue 4GB RAM 128GB ROM</v>
+      </c>
+    </row>
+    <row r="17">
+      <c r="A17" t="str">
+        <v>Samsung Galaxy M15 5G (Blue Topaz,4GB RAM,128GB Storage)| 50MP Triple Cam| 6000mAh Battery| MediaTek Dimensity 6100+ | 4 Gen. OS Upgrade &amp; 5 Year Security Update| Super AMOLED Display</v>
       </c>
     </row>
   </sheetData>
   <ignoredErrors>
-    <ignoredError numberStoredAsText="1" sqref="A1:B11"/>
+    <ignoredError numberStoredAsText="1" sqref="A1:A17"/>
   </ignoredErrors>
 </worksheet>
 </file>
</xml_diff>